<commit_message>
Removed redundant analysis directories and duplicate files
</commit_message>
<xml_diff>
--- a/lighthouse_scores_optimized.xlsx
+++ b/lighthouse_scores_optimized.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:R100"/>
+  <dimension ref="A1:Y100"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -524,6 +524,41 @@
           <t>A11y_Issue_Reduce_unused_JavaScript</t>
         </is>
       </c>
+      <c r="S1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_`[aria_hidden=""true""]`_elements_do_not_contain_focusable_descendents</t>
+        </is>
+      </c>
+      <c r="T1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_Elements_with_the_`role=text`_attribute_do_not_have_focusable_descendents</t>
+        </is>
+      </c>
+      <c r="U1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_Skip_links_are_focusable</t>
+        </is>
+      </c>
+      <c r="V1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_Skip_links_are_not_focusable</t>
+        </is>
+      </c>
+      <c r="W1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_User_focus_is_not_accidentally_trapped_in_a_region</t>
+        </is>
+      </c>
+      <c r="X1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_Interactive_controls_are_keyboard_focusable</t>
+        </is>
+      </c>
+      <c r="Y1" s="1" t="inlineStr">
+        <is>
+          <t>Accessibility_Keyboard_Focus_The_user's_focus_is_directed_to_new_content_added_to_the_page</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="n">
@@ -588,6 +623,13 @@
         <v>0.5</v>
       </c>
       <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
+      <c r="U2" t="inlineStr"/>
+      <c r="V2" t="inlineStr"/>
+      <c r="W2" t="inlineStr"/>
+      <c r="X2" t="inlineStr"/>
+      <c r="Y2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -654,6 +696,13 @@
       <c r="R3" t="n">
         <v>0</v>
       </c>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
+      <c r="U3" t="inlineStr"/>
+      <c r="V3" t="inlineStr"/>
+      <c r="W3" t="inlineStr"/>
+      <c r="X3" t="inlineStr"/>
+      <c r="Y3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -718,6 +767,13 @@
         <v>0.5</v>
       </c>
       <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
+      <c r="U4" t="inlineStr"/>
+      <c r="V4" t="inlineStr"/>
+      <c r="W4" t="inlineStr"/>
+      <c r="X4" t="inlineStr"/>
+      <c r="Y4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -784,6 +840,13 @@
       <c r="R5" t="n">
         <v>0</v>
       </c>
+      <c r="S5" t="inlineStr"/>
+      <c r="T5" t="inlineStr"/>
+      <c r="U5" t="inlineStr"/>
+      <c r="V5" t="inlineStr"/>
+      <c r="W5" t="inlineStr"/>
+      <c r="X5" t="inlineStr"/>
+      <c r="Y5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -850,6 +913,13 @@
       <c r="R6" t="n">
         <v>0</v>
       </c>
+      <c r="S6" t="inlineStr"/>
+      <c r="T6" t="inlineStr"/>
+      <c r="U6" t="inlineStr"/>
+      <c r="V6" t="inlineStr"/>
+      <c r="W6" t="inlineStr"/>
+      <c r="X6" t="inlineStr"/>
+      <c r="Y6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -890,6 +960,13 @@
       <c r="P7" t="inlineStr"/>
       <c r="Q7" t="inlineStr"/>
       <c r="R7" t="inlineStr"/>
+      <c r="S7" t="inlineStr"/>
+      <c r="T7" t="inlineStr"/>
+      <c r="U7" t="inlineStr"/>
+      <c r="V7" t="inlineStr"/>
+      <c r="W7" t="inlineStr"/>
+      <c r="X7" t="inlineStr"/>
+      <c r="Y7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -956,6 +1033,13 @@
       <c r="R8" t="n">
         <v>0</v>
       </c>
+      <c r="S8" t="inlineStr"/>
+      <c r="T8" t="inlineStr"/>
+      <c r="U8" t="inlineStr"/>
+      <c r="V8" t="inlineStr"/>
+      <c r="W8" t="inlineStr"/>
+      <c r="X8" t="inlineStr"/>
+      <c r="Y8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -1022,6 +1106,13 @@
       <c r="R9" t="n">
         <v>0</v>
       </c>
+      <c r="S9" t="inlineStr"/>
+      <c r="T9" t="inlineStr"/>
+      <c r="U9" t="inlineStr"/>
+      <c r="V9" t="inlineStr"/>
+      <c r="W9" t="inlineStr"/>
+      <c r="X9" t="inlineStr"/>
+      <c r="Y9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -1088,6 +1179,13 @@
       <c r="R10" t="n">
         <v>0</v>
       </c>
+      <c r="S10" t="inlineStr"/>
+      <c r="T10" t="inlineStr"/>
+      <c r="U10" t="inlineStr"/>
+      <c r="V10" t="inlineStr"/>
+      <c r="W10" t="inlineStr"/>
+      <c r="X10" t="inlineStr"/>
+      <c r="Y10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -1154,6 +1252,13 @@
       <c r="R11" t="n">
         <v>0</v>
       </c>
+      <c r="S11" t="inlineStr"/>
+      <c r="T11" t="inlineStr"/>
+      <c r="U11" t="inlineStr"/>
+      <c r="V11" t="inlineStr"/>
+      <c r="W11" t="inlineStr"/>
+      <c r="X11" t="inlineStr"/>
+      <c r="Y11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -1220,6 +1325,13 @@
       <c r="R12" t="n">
         <v>0</v>
       </c>
+      <c r="S12" t="inlineStr"/>
+      <c r="T12" t="inlineStr"/>
+      <c r="U12" t="inlineStr"/>
+      <c r="V12" t="inlineStr"/>
+      <c r="W12" t="inlineStr"/>
+      <c r="X12" t="inlineStr"/>
+      <c r="Y12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -1286,6 +1398,13 @@
       <c r="R13" t="n">
         <v>0</v>
       </c>
+      <c r="S13" t="inlineStr"/>
+      <c r="T13" t="inlineStr"/>
+      <c r="U13" t="inlineStr"/>
+      <c r="V13" t="inlineStr"/>
+      <c r="W13" t="inlineStr"/>
+      <c r="X13" t="inlineStr"/>
+      <c r="Y13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -1326,6 +1445,13 @@
       <c r="P14" t="inlineStr"/>
       <c r="Q14" t="inlineStr"/>
       <c r="R14" t="inlineStr"/>
+      <c r="S14" t="inlineStr"/>
+      <c r="T14" t="inlineStr"/>
+      <c r="U14" t="inlineStr"/>
+      <c r="V14" t="inlineStr"/>
+      <c r="W14" t="inlineStr"/>
+      <c r="X14" t="inlineStr"/>
+      <c r="Y14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1392,6 +1518,13 @@
       <c r="R15" t="n">
         <v>0</v>
       </c>
+      <c r="S15" t="inlineStr"/>
+      <c r="T15" t="inlineStr"/>
+      <c r="U15" t="inlineStr"/>
+      <c r="V15" t="inlineStr"/>
+      <c r="W15" t="inlineStr"/>
+      <c r="X15" t="inlineStr"/>
+      <c r="Y15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1456,6 +1589,13 @@
       <c r="R16" t="n">
         <v>0</v>
       </c>
+      <c r="S16" t="inlineStr"/>
+      <c r="T16" t="inlineStr"/>
+      <c r="U16" t="inlineStr"/>
+      <c r="V16" t="inlineStr"/>
+      <c r="W16" t="inlineStr"/>
+      <c r="X16" t="inlineStr"/>
+      <c r="Y16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1522,6 +1662,13 @@
       <c r="R17" t="n">
         <v>0</v>
       </c>
+      <c r="S17" t="inlineStr"/>
+      <c r="T17" t="inlineStr"/>
+      <c r="U17" t="inlineStr"/>
+      <c r="V17" t="inlineStr"/>
+      <c r="W17" t="inlineStr"/>
+      <c r="X17" t="inlineStr"/>
+      <c r="Y17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -1588,6 +1735,13 @@
       <c r="R18" t="n">
         <v>0</v>
       </c>
+      <c r="S18" t="inlineStr"/>
+      <c r="T18" t="inlineStr"/>
+      <c r="U18" t="inlineStr"/>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
+      <c r="X18" t="inlineStr"/>
+      <c r="Y18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="n">
@@ -1654,6 +1808,13 @@
       <c r="R19" t="n">
         <v>0</v>
       </c>
+      <c r="S19" t="inlineStr"/>
+      <c r="T19" t="inlineStr"/>
+      <c r="U19" t="inlineStr"/>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
+      <c r="X19" t="inlineStr"/>
+      <c r="Y19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="n">
@@ -1720,6 +1881,13 @@
       <c r="R20" t="n">
         <v>0</v>
       </c>
+      <c r="S20" t="inlineStr"/>
+      <c r="T20" t="inlineStr"/>
+      <c r="U20" t="inlineStr"/>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
+      <c r="X20" t="inlineStr"/>
+      <c r="Y20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="n">
@@ -1786,6 +1954,13 @@
       <c r="R21" t="n">
         <v>0</v>
       </c>
+      <c r="S21" t="inlineStr"/>
+      <c r="T21" t="inlineStr"/>
+      <c r="U21" t="inlineStr"/>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
+      <c r="X21" t="inlineStr"/>
+      <c r="Y21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="n">
@@ -1852,6 +2027,13 @@
       <c r="R22" t="n">
         <v>0</v>
       </c>
+      <c r="S22" t="inlineStr"/>
+      <c r="T22" t="inlineStr"/>
+      <c r="U22" t="inlineStr"/>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
+      <c r="X22" t="inlineStr"/>
+      <c r="Y22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="n">
@@ -1916,6 +2098,13 @@
       <c r="R23" t="n">
         <v>0</v>
       </c>
+      <c r="S23" t="inlineStr"/>
+      <c r="T23" t="inlineStr"/>
+      <c r="U23" t="inlineStr"/>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
+      <c r="X23" t="inlineStr"/>
+      <c r="Y23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="n">
@@ -1982,6 +2171,13 @@
       <c r="R24" t="n">
         <v>0</v>
       </c>
+      <c r="S24" t="inlineStr"/>
+      <c r="T24" t="inlineStr"/>
+      <c r="U24" t="inlineStr"/>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
+      <c r="X24" t="inlineStr"/>
+      <c r="Y24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="n">
@@ -2022,6 +2218,13 @@
       <c r="P25" t="inlineStr"/>
       <c r="Q25" t="inlineStr"/>
       <c r="R25" t="inlineStr"/>
+      <c r="S25" t="inlineStr"/>
+      <c r="T25" t="inlineStr"/>
+      <c r="U25" t="inlineStr"/>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
+      <c r="X25" t="inlineStr"/>
+      <c r="Y25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="n">
@@ -2086,6 +2289,13 @@
       <c r="R26" t="n">
         <v>0</v>
       </c>
+      <c r="S26" t="inlineStr"/>
+      <c r="T26" t="inlineStr"/>
+      <c r="U26" t="inlineStr"/>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
+      <c r="X26" t="inlineStr"/>
+      <c r="Y26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -2152,6 +2362,13 @@
       <c r="R27" t="n">
         <v>0</v>
       </c>
+      <c r="S27" t="inlineStr"/>
+      <c r="T27" t="inlineStr"/>
+      <c r="U27" t="inlineStr"/>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
+      <c r="X27" t="inlineStr"/>
+      <c r="Y27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="n">
@@ -2218,6 +2435,15 @@
       <c r="R28" t="n">
         <v>0</v>
       </c>
+      <c r="S28" t="inlineStr"/>
+      <c r="T28" t="inlineStr"/>
+      <c r="U28" t="inlineStr"/>
+      <c r="V28" t="n">
+        <v>0</v>
+      </c>
+      <c r="W28" t="inlineStr"/>
+      <c r="X28" t="inlineStr"/>
+      <c r="Y28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="n">
@@ -2284,6 +2510,13 @@
       <c r="R29" t="n">
         <v>0</v>
       </c>
+      <c r="S29" t="inlineStr"/>
+      <c r="T29" t="inlineStr"/>
+      <c r="U29" t="inlineStr"/>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
+      <c r="X29" t="inlineStr"/>
+      <c r="Y29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="n">
@@ -2348,6 +2581,13 @@
       <c r="R30" t="n">
         <v>0</v>
       </c>
+      <c r="S30" t="inlineStr"/>
+      <c r="T30" t="inlineStr"/>
+      <c r="U30" t="inlineStr"/>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
+      <c r="X30" t="inlineStr"/>
+      <c r="Y30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="n">
@@ -2414,6 +2654,13 @@
       <c r="R31" t="n">
         <v>0.5</v>
       </c>
+      <c r="S31" t="inlineStr"/>
+      <c r="T31" t="inlineStr"/>
+      <c r="U31" t="inlineStr"/>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
+      <c r="X31" t="inlineStr"/>
+      <c r="Y31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="n">
@@ -2454,6 +2701,13 @@
       <c r="P32" t="inlineStr"/>
       <c r="Q32" t="inlineStr"/>
       <c r="R32" t="inlineStr"/>
+      <c r="S32" t="inlineStr"/>
+      <c r="T32" t="inlineStr"/>
+      <c r="U32" t="inlineStr"/>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
+      <c r="X32" t="inlineStr"/>
+      <c r="Y32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="n">
@@ -2520,6 +2774,13 @@
       <c r="R33" t="n">
         <v>0</v>
       </c>
+      <c r="S33" t="inlineStr"/>
+      <c r="T33" t="inlineStr"/>
+      <c r="U33" t="inlineStr"/>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
+      <c r="X33" t="inlineStr"/>
+      <c r="Y33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="n">
@@ -2586,6 +2847,13 @@
       <c r="R34" t="n">
         <v>0</v>
       </c>
+      <c r="S34" t="inlineStr"/>
+      <c r="T34" t="inlineStr"/>
+      <c r="U34" t="inlineStr"/>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
+      <c r="X34" t="inlineStr"/>
+      <c r="Y34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="n">
@@ -2652,6 +2920,13 @@
       <c r="R35" t="n">
         <v>0.5</v>
       </c>
+      <c r="S35" t="inlineStr"/>
+      <c r="T35" t="inlineStr"/>
+      <c r="U35" t="inlineStr"/>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
+      <c r="X35" t="inlineStr"/>
+      <c r="Y35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="n">
@@ -2718,6 +2993,13 @@
       <c r="R36" t="n">
         <v>0</v>
       </c>
+      <c r="S36" t="inlineStr"/>
+      <c r="T36" t="inlineStr"/>
+      <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
+      <c r="X36" t="inlineStr"/>
+      <c r="Y36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="n">
@@ -2758,6 +3040,13 @@
       <c r="P37" t="inlineStr"/>
       <c r="Q37" t="inlineStr"/>
       <c r="R37" t="inlineStr"/>
+      <c r="S37" t="inlineStr"/>
+      <c r="T37" t="inlineStr"/>
+      <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
+      <c r="X37" t="inlineStr"/>
+      <c r="Y37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="n">
@@ -2824,6 +3113,13 @@
       <c r="R38" t="n">
         <v>0</v>
       </c>
+      <c r="S38" t="inlineStr"/>
+      <c r="T38" t="inlineStr"/>
+      <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
+      <c r="X38" t="inlineStr"/>
+      <c r="Y38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="n">
@@ -2864,6 +3160,13 @@
       <c r="P39" t="inlineStr"/>
       <c r="Q39" t="inlineStr"/>
       <c r="R39" t="inlineStr"/>
+      <c r="S39" t="inlineStr"/>
+      <c r="T39" t="inlineStr"/>
+      <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
+      <c r="X39" t="inlineStr"/>
+      <c r="Y39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -2930,6 +3233,13 @@
       <c r="R40" t="n">
         <v>0</v>
       </c>
+      <c r="S40" t="inlineStr"/>
+      <c r="T40" t="inlineStr"/>
+      <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
+      <c r="X40" t="inlineStr"/>
+      <c r="Y40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="n">
@@ -2996,6 +3306,13 @@
       <c r="R41" t="n">
         <v>0</v>
       </c>
+      <c r="S41" t="inlineStr"/>
+      <c r="T41" t="inlineStr"/>
+      <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
+      <c r="X41" t="inlineStr"/>
+      <c r="Y41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="n">
@@ -3062,6 +3379,13 @@
       <c r="R42" t="n">
         <v>0</v>
       </c>
+      <c r="S42" t="inlineStr"/>
+      <c r="T42" t="inlineStr"/>
+      <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
+      <c r="X42" t="inlineStr"/>
+      <c r="Y42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="n">
@@ -3128,6 +3452,13 @@
       <c r="R43" t="n">
         <v>0</v>
       </c>
+      <c r="S43" t="inlineStr"/>
+      <c r="T43" t="inlineStr"/>
+      <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
+      <c r="X43" t="inlineStr"/>
+      <c r="Y43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="n">
@@ -3194,6 +3525,13 @@
       <c r="R44" t="n">
         <v>0</v>
       </c>
+      <c r="S44" t="inlineStr"/>
+      <c r="T44" t="inlineStr"/>
+      <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
+      <c r="X44" t="inlineStr"/>
+      <c r="Y44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="n">
@@ -3260,6 +3598,13 @@
       <c r="R45" t="n">
         <v>0</v>
       </c>
+      <c r="S45" t="inlineStr"/>
+      <c r="T45" t="inlineStr"/>
+      <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
+      <c r="X45" t="inlineStr"/>
+      <c r="Y45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -3326,6 +3671,13 @@
       <c r="R46" t="n">
         <v>0</v>
       </c>
+      <c r="S46" t="inlineStr"/>
+      <c r="T46" t="inlineStr"/>
+      <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
+      <c r="X46" t="inlineStr"/>
+      <c r="Y46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="n">
@@ -3392,6 +3744,13 @@
       <c r="R47" t="n">
         <v>0</v>
       </c>
+      <c r="S47" t="inlineStr"/>
+      <c r="T47" t="inlineStr"/>
+      <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
+      <c r="X47" t="inlineStr"/>
+      <c r="Y47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="n">
@@ -3456,6 +3815,13 @@
         <v>0.5</v>
       </c>
       <c r="R48" t="inlineStr"/>
+      <c r="S48" t="inlineStr"/>
+      <c r="T48" t="inlineStr"/>
+      <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
+      <c r="X48" t="inlineStr"/>
+      <c r="Y48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="n">
@@ -3516,6 +3882,13 @@
         <v>0</v>
       </c>
       <c r="R49" t="inlineStr"/>
+      <c r="S49" t="inlineStr"/>
+      <c r="T49" t="inlineStr"/>
+      <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
+      <c r="X49" t="inlineStr"/>
+      <c r="Y49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="n">
@@ -3582,6 +3955,13 @@
       <c r="R50" t="n">
         <v>0</v>
       </c>
+      <c r="S50" t="inlineStr"/>
+      <c r="T50" t="inlineStr"/>
+      <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
+      <c r="X50" t="inlineStr"/>
+      <c r="Y50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -3646,6 +4026,13 @@
         <v>0.5</v>
       </c>
       <c r="R51" t="inlineStr"/>
+      <c r="S51" t="inlineStr"/>
+      <c r="T51" t="inlineStr"/>
+      <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
+      <c r="X51" t="inlineStr"/>
+      <c r="Y51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="n">
@@ -3712,6 +4099,13 @@
       <c r="R52" t="n">
         <v>0.5</v>
       </c>
+      <c r="S52" t="inlineStr"/>
+      <c r="T52" t="inlineStr"/>
+      <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
+      <c r="X52" t="inlineStr"/>
+      <c r="Y52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="n">
@@ -3778,6 +4172,13 @@
       <c r="R53" t="n">
         <v>0</v>
       </c>
+      <c r="S53" t="inlineStr"/>
+      <c r="T53" t="inlineStr"/>
+      <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
+      <c r="X53" t="inlineStr"/>
+      <c r="Y53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="n">
@@ -3842,6 +4243,13 @@
       <c r="R54" t="n">
         <v>0.5</v>
       </c>
+      <c r="S54" t="inlineStr"/>
+      <c r="T54" t="inlineStr"/>
+      <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
+      <c r="X54" t="inlineStr"/>
+      <c r="Y54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="n">
@@ -3908,6 +4316,13 @@
       <c r="R55" t="n">
         <v>0.5</v>
       </c>
+      <c r="S55" t="inlineStr"/>
+      <c r="T55" t="inlineStr"/>
+      <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
+      <c r="X55" t="inlineStr"/>
+      <c r="Y55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="n">
@@ -3974,6 +4389,13 @@
       <c r="R56" t="n">
         <v>0</v>
       </c>
+      <c r="S56" t="inlineStr"/>
+      <c r="T56" t="inlineStr"/>
+      <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
+      <c r="X56" t="inlineStr"/>
+      <c r="Y56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="n">
@@ -4040,6 +4462,13 @@
       <c r="R57" t="n">
         <v>0</v>
       </c>
+      <c r="S57" t="inlineStr"/>
+      <c r="T57" t="inlineStr"/>
+      <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
+      <c r="X57" t="inlineStr"/>
+      <c r="Y57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="n">
@@ -4100,6 +4529,13 @@
       <c r="P58" t="inlineStr"/>
       <c r="Q58" t="inlineStr"/>
       <c r="R58" t="inlineStr"/>
+      <c r="S58" t="inlineStr"/>
+      <c r="T58" t="inlineStr"/>
+      <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
+      <c r="X58" t="inlineStr"/>
+      <c r="Y58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="n">
@@ -4166,6 +4602,13 @@
       <c r="R59" t="n">
         <v>0</v>
       </c>
+      <c r="S59" t="inlineStr"/>
+      <c r="T59" t="inlineStr"/>
+      <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
+      <c r="X59" t="inlineStr"/>
+      <c r="Y59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="n">
@@ -4232,6 +4675,13 @@
       <c r="R60" t="n">
         <v>0</v>
       </c>
+      <c r="S60" t="inlineStr"/>
+      <c r="T60" t="inlineStr"/>
+      <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
+      <c r="X60" t="inlineStr"/>
+      <c r="Y60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="n">
@@ -4298,6 +4748,13 @@
       <c r="R61" t="n">
         <v>0</v>
       </c>
+      <c r="S61" t="inlineStr"/>
+      <c r="T61" t="inlineStr"/>
+      <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
+      <c r="X61" t="inlineStr"/>
+      <c r="Y61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -4364,6 +4821,13 @@
       <c r="R62" t="n">
         <v>0</v>
       </c>
+      <c r="S62" t="inlineStr"/>
+      <c r="T62" t="inlineStr"/>
+      <c r="U62" t="inlineStr"/>
+      <c r="V62" t="inlineStr"/>
+      <c r="W62" t="inlineStr"/>
+      <c r="X62" t="inlineStr"/>
+      <c r="Y62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="n">
@@ -4430,6 +4894,13 @@
       <c r="R63" t="n">
         <v>0</v>
       </c>
+      <c r="S63" t="inlineStr"/>
+      <c r="T63" t="inlineStr"/>
+      <c r="U63" t="inlineStr"/>
+      <c r="V63" t="inlineStr"/>
+      <c r="W63" t="inlineStr"/>
+      <c r="X63" t="inlineStr"/>
+      <c r="Y63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="n">
@@ -4496,6 +4967,15 @@
       <c r="R64" t="n">
         <v>0</v>
       </c>
+      <c r="S64" t="inlineStr"/>
+      <c r="T64" t="inlineStr"/>
+      <c r="U64" t="inlineStr"/>
+      <c r="V64" t="n">
+        <v>0</v>
+      </c>
+      <c r="W64" t="inlineStr"/>
+      <c r="X64" t="inlineStr"/>
+      <c r="Y64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -4562,6 +5042,13 @@
       <c r="R65" t="n">
         <v>0</v>
       </c>
+      <c r="S65" t="inlineStr"/>
+      <c r="T65" t="inlineStr"/>
+      <c r="U65" t="inlineStr"/>
+      <c r="V65" t="inlineStr"/>
+      <c r="W65" t="inlineStr"/>
+      <c r="X65" t="inlineStr"/>
+      <c r="Y65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="n">
@@ -4628,6 +5115,13 @@
       <c r="R66" t="n">
         <v>0</v>
       </c>
+      <c r="S66" t="inlineStr"/>
+      <c r="T66" t="inlineStr"/>
+      <c r="U66" t="inlineStr"/>
+      <c r="V66" t="inlineStr"/>
+      <c r="W66" t="inlineStr"/>
+      <c r="X66" t="inlineStr"/>
+      <c r="Y66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="n">
@@ -4694,6 +5188,13 @@
       <c r="R67" t="n">
         <v>0</v>
       </c>
+      <c r="S67" t="inlineStr"/>
+      <c r="T67" t="inlineStr"/>
+      <c r="U67" t="inlineStr"/>
+      <c r="V67" t="inlineStr"/>
+      <c r="W67" t="inlineStr"/>
+      <c r="X67" t="inlineStr"/>
+      <c r="Y67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="n">
@@ -4760,6 +5261,13 @@
       <c r="R68" t="n">
         <v>0</v>
       </c>
+      <c r="S68" t="inlineStr"/>
+      <c r="T68" t="inlineStr"/>
+      <c r="U68" t="inlineStr"/>
+      <c r="V68" t="inlineStr"/>
+      <c r="W68" t="inlineStr"/>
+      <c r="X68" t="inlineStr"/>
+      <c r="Y68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -4826,6 +5334,13 @@
       <c r="R69" t="n">
         <v>0</v>
       </c>
+      <c r="S69" t="inlineStr"/>
+      <c r="T69" t="inlineStr"/>
+      <c r="U69" t="inlineStr"/>
+      <c r="V69" t="inlineStr"/>
+      <c r="W69" t="inlineStr"/>
+      <c r="X69" t="inlineStr"/>
+      <c r="Y69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="n">
@@ -4890,6 +5405,13 @@
       <c r="R70" t="n">
         <v>0.5</v>
       </c>
+      <c r="S70" t="inlineStr"/>
+      <c r="T70" t="inlineStr"/>
+      <c r="U70" t="inlineStr"/>
+      <c r="V70" t="inlineStr"/>
+      <c r="W70" t="inlineStr"/>
+      <c r="X70" t="inlineStr"/>
+      <c r="Y70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -4956,6 +5478,13 @@
       <c r="R71" t="n">
         <v>0</v>
       </c>
+      <c r="S71" t="inlineStr"/>
+      <c r="T71" t="inlineStr"/>
+      <c r="U71" t="inlineStr"/>
+      <c r="V71" t="inlineStr"/>
+      <c r="W71" t="inlineStr"/>
+      <c r="X71" t="inlineStr"/>
+      <c r="Y71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="n">
@@ -5020,6 +5549,13 @@
       <c r="R72" t="n">
         <v>0</v>
       </c>
+      <c r="S72" t="inlineStr"/>
+      <c r="T72" t="inlineStr"/>
+      <c r="U72" t="inlineStr"/>
+      <c r="V72" t="inlineStr"/>
+      <c r="W72" t="inlineStr"/>
+      <c r="X72" t="inlineStr"/>
+      <c r="Y72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="n">
@@ -5086,6 +5622,13 @@
       <c r="R73" t="n">
         <v>0</v>
       </c>
+      <c r="S73" t="inlineStr"/>
+      <c r="T73" t="inlineStr"/>
+      <c r="U73" t="inlineStr"/>
+      <c r="V73" t="inlineStr"/>
+      <c r="W73" t="inlineStr"/>
+      <c r="X73" t="inlineStr"/>
+      <c r="Y73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="n">
@@ -5152,6 +5695,13 @@
       <c r="R74" t="n">
         <v>0</v>
       </c>
+      <c r="S74" t="inlineStr"/>
+      <c r="T74" t="inlineStr"/>
+      <c r="U74" t="inlineStr"/>
+      <c r="V74" t="inlineStr"/>
+      <c r="W74" t="inlineStr"/>
+      <c r="X74" t="inlineStr"/>
+      <c r="Y74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="n">
@@ -5218,6 +5768,13 @@
       <c r="R75" t="n">
         <v>0</v>
       </c>
+      <c r="S75" t="inlineStr"/>
+      <c r="T75" t="inlineStr"/>
+      <c r="U75" t="inlineStr"/>
+      <c r="V75" t="inlineStr"/>
+      <c r="W75" t="inlineStr"/>
+      <c r="X75" t="inlineStr"/>
+      <c r="Y75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="n">
@@ -5284,6 +5841,13 @@
       <c r="R76" t="n">
         <v>0</v>
       </c>
+      <c r="S76" t="inlineStr"/>
+      <c r="T76" t="inlineStr"/>
+      <c r="U76" t="inlineStr"/>
+      <c r="V76" t="inlineStr"/>
+      <c r="W76" t="inlineStr"/>
+      <c r="X76" t="inlineStr"/>
+      <c r="Y76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="n">
@@ -5350,6 +5914,13 @@
       <c r="R77" t="n">
         <v>0</v>
       </c>
+      <c r="S77" t="inlineStr"/>
+      <c r="T77" t="inlineStr"/>
+      <c r="U77" t="inlineStr"/>
+      <c r="V77" t="inlineStr"/>
+      <c r="W77" t="inlineStr"/>
+      <c r="X77" t="inlineStr"/>
+      <c r="Y77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="n">
@@ -5410,6 +5981,13 @@
       <c r="R78" t="n">
         <v>0.5</v>
       </c>
+      <c r="S78" t="inlineStr"/>
+      <c r="T78" t="inlineStr"/>
+      <c r="U78" t="inlineStr"/>
+      <c r="V78" t="inlineStr"/>
+      <c r="W78" t="inlineStr"/>
+      <c r="X78" t="inlineStr"/>
+      <c r="Y78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="n">
@@ -5476,6 +6054,13 @@
       <c r="R79" t="n">
         <v>0.5</v>
       </c>
+      <c r="S79" t="inlineStr"/>
+      <c r="T79" t="inlineStr"/>
+      <c r="U79" t="inlineStr"/>
+      <c r="V79" t="inlineStr"/>
+      <c r="W79" t="inlineStr"/>
+      <c r="X79" t="inlineStr"/>
+      <c r="Y79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -5542,6 +6127,13 @@
       <c r="R80" t="n">
         <v>0</v>
       </c>
+      <c r="S80" t="inlineStr"/>
+      <c r="T80" t="inlineStr"/>
+      <c r="U80" t="inlineStr"/>
+      <c r="V80" t="inlineStr"/>
+      <c r="W80" t="inlineStr"/>
+      <c r="X80" t="inlineStr"/>
+      <c r="Y80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="n">
@@ -5608,6 +6200,13 @@
       <c r="R81" t="n">
         <v>0</v>
       </c>
+      <c r="S81" t="inlineStr"/>
+      <c r="T81" t="inlineStr"/>
+      <c r="U81" t="inlineStr"/>
+      <c r="V81" t="inlineStr"/>
+      <c r="W81" t="inlineStr"/>
+      <c r="X81" t="inlineStr"/>
+      <c r="Y81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="n">
@@ -5670,6 +6269,13 @@
       </c>
       <c r="Q82" t="inlineStr"/>
       <c r="R82" t="inlineStr"/>
+      <c r="S82" t="inlineStr"/>
+      <c r="T82" t="inlineStr"/>
+      <c r="U82" t="inlineStr"/>
+      <c r="V82" t="inlineStr"/>
+      <c r="W82" t="inlineStr"/>
+      <c r="X82" t="inlineStr"/>
+      <c r="Y82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -5734,6 +6340,13 @@
       <c r="R83" t="n">
         <v>0.5</v>
       </c>
+      <c r="S83" t="inlineStr"/>
+      <c r="T83" t="inlineStr"/>
+      <c r="U83" t="inlineStr"/>
+      <c r="V83" t="inlineStr"/>
+      <c r="W83" t="inlineStr"/>
+      <c r="X83" t="inlineStr"/>
+      <c r="Y83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -5800,6 +6413,13 @@
       <c r="R84" t="n">
         <v>0</v>
       </c>
+      <c r="S84" t="inlineStr"/>
+      <c r="T84" t="inlineStr"/>
+      <c r="U84" t="inlineStr"/>
+      <c r="V84" t="inlineStr"/>
+      <c r="W84" t="inlineStr"/>
+      <c r="X84" t="inlineStr"/>
+      <c r="Y84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="n">
@@ -5866,6 +6486,13 @@
       <c r="R85" t="n">
         <v>0</v>
       </c>
+      <c r="S85" t="inlineStr"/>
+      <c r="T85" t="inlineStr"/>
+      <c r="U85" t="inlineStr"/>
+      <c r="V85" t="inlineStr"/>
+      <c r="W85" t="inlineStr"/>
+      <c r="X85" t="inlineStr"/>
+      <c r="Y85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="n">
@@ -5930,6 +6557,13 @@
       <c r="R86" t="n">
         <v>0</v>
       </c>
+      <c r="S86" t="inlineStr"/>
+      <c r="T86" t="inlineStr"/>
+      <c r="U86" t="inlineStr"/>
+      <c r="V86" t="inlineStr"/>
+      <c r="W86" t="inlineStr"/>
+      <c r="X86" t="inlineStr"/>
+      <c r="Y86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -5996,6 +6630,13 @@
       <c r="R87" t="n">
         <v>0</v>
       </c>
+      <c r="S87" t="inlineStr"/>
+      <c r="T87" t="inlineStr"/>
+      <c r="U87" t="inlineStr"/>
+      <c r="V87" t="inlineStr"/>
+      <c r="W87" t="inlineStr"/>
+      <c r="X87" t="inlineStr"/>
+      <c r="Y87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="n">
@@ -6062,6 +6703,13 @@
       <c r="R88" t="n">
         <v>0</v>
       </c>
+      <c r="S88" t="inlineStr"/>
+      <c r="T88" t="inlineStr"/>
+      <c r="U88" t="inlineStr"/>
+      <c r="V88" t="inlineStr"/>
+      <c r="W88" t="inlineStr"/>
+      <c r="X88" t="inlineStr"/>
+      <c r="Y88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="n">
@@ -6126,6 +6774,13 @@
       <c r="R89" t="n">
         <v>0</v>
       </c>
+      <c r="S89" t="inlineStr"/>
+      <c r="T89" t="inlineStr"/>
+      <c r="U89" t="inlineStr"/>
+      <c r="V89" t="inlineStr"/>
+      <c r="W89" t="inlineStr"/>
+      <c r="X89" t="inlineStr"/>
+      <c r="Y89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="n">
@@ -6192,6 +6847,13 @@
       <c r="R90" t="n">
         <v>0</v>
       </c>
+      <c r="S90" t="inlineStr"/>
+      <c r="T90" t="inlineStr"/>
+      <c r="U90" t="inlineStr"/>
+      <c r="V90" t="inlineStr"/>
+      <c r="W90" t="inlineStr"/>
+      <c r="X90" t="inlineStr"/>
+      <c r="Y90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="n">
@@ -6232,6 +6894,13 @@
       <c r="P91" t="inlineStr"/>
       <c r="Q91" t="inlineStr"/>
       <c r="R91" t="inlineStr"/>
+      <c r="S91" t="inlineStr"/>
+      <c r="T91" t="inlineStr"/>
+      <c r="U91" t="inlineStr"/>
+      <c r="V91" t="inlineStr"/>
+      <c r="W91" t="inlineStr"/>
+      <c r="X91" t="inlineStr"/>
+      <c r="Y91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="n">
@@ -6298,6 +6967,13 @@
       <c r="R92" t="n">
         <v>0</v>
       </c>
+      <c r="S92" t="inlineStr"/>
+      <c r="T92" t="inlineStr"/>
+      <c r="U92" t="inlineStr"/>
+      <c r="V92" t="inlineStr"/>
+      <c r="W92" t="inlineStr"/>
+      <c r="X92" t="inlineStr"/>
+      <c r="Y92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="n">
@@ -6364,6 +7040,13 @@
       <c r="R93" t="n">
         <v>0</v>
       </c>
+      <c r="S93" t="inlineStr"/>
+      <c r="T93" t="inlineStr"/>
+      <c r="U93" t="inlineStr"/>
+      <c r="V93" t="inlineStr"/>
+      <c r="W93" t="inlineStr"/>
+      <c r="X93" t="inlineStr"/>
+      <c r="Y93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="n">
@@ -6430,6 +7113,13 @@
       <c r="R94" t="n">
         <v>0</v>
       </c>
+      <c r="S94" t="inlineStr"/>
+      <c r="T94" t="inlineStr"/>
+      <c r="U94" t="inlineStr"/>
+      <c r="V94" t="inlineStr"/>
+      <c r="W94" t="inlineStr"/>
+      <c r="X94" t="inlineStr"/>
+      <c r="Y94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="n">
@@ -6494,6 +7184,13 @@
         <v>0</v>
       </c>
       <c r="R95" t="inlineStr"/>
+      <c r="S95" t="inlineStr"/>
+      <c r="T95" t="inlineStr"/>
+      <c r="U95" t="inlineStr"/>
+      <c r="V95" t="inlineStr"/>
+      <c r="W95" t="inlineStr"/>
+      <c r="X95" t="inlineStr"/>
+      <c r="Y95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="n">
@@ -6558,6 +7255,13 @@
         <v>0.5</v>
       </c>
       <c r="R96" t="inlineStr"/>
+      <c r="S96" t="inlineStr"/>
+      <c r="T96" t="inlineStr"/>
+      <c r="U96" t="inlineStr"/>
+      <c r="V96" t="inlineStr"/>
+      <c r="W96" t="inlineStr"/>
+      <c r="X96" t="inlineStr"/>
+      <c r="Y96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="n">
@@ -6624,6 +7328,13 @@
       <c r="R97" t="n">
         <v>0</v>
       </c>
+      <c r="S97" t="inlineStr"/>
+      <c r="T97" t="inlineStr"/>
+      <c r="U97" t="inlineStr"/>
+      <c r="V97" t="inlineStr"/>
+      <c r="W97" t="inlineStr"/>
+      <c r="X97" t="inlineStr"/>
+      <c r="Y97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="n">
@@ -6690,6 +7401,13 @@
       <c r="R98" t="n">
         <v>0</v>
       </c>
+      <c r="S98" t="inlineStr"/>
+      <c r="T98" t="inlineStr"/>
+      <c r="U98" t="inlineStr"/>
+      <c r="V98" t="inlineStr"/>
+      <c r="W98" t="inlineStr"/>
+      <c r="X98" t="inlineStr"/>
+      <c r="Y98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -6756,6 +7474,13 @@
       <c r="R99" t="n">
         <v>0</v>
       </c>
+      <c r="S99" t="inlineStr"/>
+      <c r="T99" t="inlineStr"/>
+      <c r="U99" t="inlineStr"/>
+      <c r="V99" t="inlineStr"/>
+      <c r="W99" t="inlineStr"/>
+      <c r="X99" t="inlineStr"/>
+      <c r="Y99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -6822,6 +7547,13 @@
       <c r="R100" t="n">
         <v>0</v>
       </c>
+      <c r="S100" t="inlineStr"/>
+      <c r="T100" t="inlineStr"/>
+      <c r="U100" t="inlineStr"/>
+      <c r="V100" t="inlineStr"/>
+      <c r="W100" t="inlineStr"/>
+      <c r="X100" t="inlineStr"/>
+      <c r="Y100" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>